<commit_message>
Commit logo, navbar and sub-menu
</commit_message>
<xml_diff>
--- a/Tasks.xlsx
+++ b/Tasks.xlsx
@@ -106,12 +106,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="24">
+  <fonts count="25">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -135,88 +135,32 @@
     </font>
     <font>
       <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="134"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -231,7 +175,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -245,9 +189,85 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -262,29 +282,14 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -323,37 +328,79 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -365,7 +412,67 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -377,13 +484,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -395,115 +502,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -532,16 +537,25 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
-      <right style="thin">
+      <right style="double">
         <color rgb="FF3F3F3F"/>
       </right>
-      <top style="thin">
+      <top style="double">
         <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="thin">
+      <bottom style="double">
         <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
@@ -563,6 +577,32 @@
     </border>
     <border>
       <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
@@ -573,30 +613,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -612,17 +628,6 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
@@ -634,7 +639,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -652,134 +657,134 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="13" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="24" fillId="22" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="14" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="14" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="27" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -798,28 +803,31 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
+    <xf numFmtId="16" fontId="3" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
     <xf numFmtId="16" fontId="2" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="3" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="9" fontId="4" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="16" fontId="4" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -831,10 +839,10 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="7">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="7" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
   </cellXfs>
@@ -1159,7 +1167,7 @@
   <dimension ref="A1:M17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
@@ -1200,13 +1208,13 @@
       <c r="H1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="16" t="s">
+      <c r="I1" s="17" t="s">
         <v>4</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="M1" s="17" t="s">
+      <c r="M1" s="18" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1214,96 +1222,112 @@
       <c r="A2" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="6"/>
+      <c r="B2" s="6">
+        <v>45090</v>
+      </c>
       <c r="C2" s="6"/>
-      <c r="D2" s="7"/>
+      <c r="D2" s="7">
+        <v>0.6</v>
+      </c>
       <c r="E2" s="8" t="s">
         <v>11</v>
       </c>
       <c r="F2" s="8"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="9"/>
-      <c r="I2" s="18"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="10"/>
+      <c r="I2" s="19"/>
       <c r="J2" s="8"/>
     </row>
     <row r="3" spans="1:10">
       <c r="A3" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="8"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="10"/>
+      <c r="B3" s="6">
+        <v>45090</v>
+      </c>
+      <c r="C3" s="6"/>
+      <c r="D3" s="11">
+        <v>0.6</v>
+      </c>
       <c r="E3" s="8" t="s">
         <v>11</v>
       </c>
       <c r="F3" s="8"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="10"/>
-      <c r="I3" s="18"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="11"/>
+      <c r="I3" s="19"/>
       <c r="J3" s="8"/>
     </row>
     <row r="4" spans="1:10">
       <c r="A4" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="6"/>
+      <c r="B4" s="6">
+        <v>45090</v>
+      </c>
       <c r="C4" s="6"/>
-      <c r="D4" s="11"/>
+      <c r="D4" s="12">
+        <v>0.6</v>
+      </c>
       <c r="E4" s="8" t="s">
         <v>11</v>
       </c>
       <c r="F4" s="8"/>
-      <c r="G4" s="6"/>
-      <c r="H4" s="11"/>
-      <c r="I4" s="18"/>
+      <c r="G4" s="9"/>
+      <c r="H4" s="12"/>
+      <c r="I4" s="19"/>
       <c r="J4" s="8"/>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="12"/>
-      <c r="C5" s="12"/>
-      <c r="D5" s="7"/>
+      <c r="B5" s="6">
+        <v>45090</v>
+      </c>
+      <c r="C5" s="6"/>
+      <c r="D5" s="12">
+        <v>0.6</v>
+      </c>
       <c r="E5" s="8" t="s">
         <v>11</v>
       </c>
       <c r="F5" s="8"/>
-      <c r="G5" s="6"/>
-      <c r="H5" s="7"/>
-      <c r="I5" s="18"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="13"/>
+      <c r="I5" s="19"/>
       <c r="J5" s="8"/>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="12"/>
-      <c r="C6" s="12"/>
-      <c r="D6" s="11"/>
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="12"/>
       <c r="E6" s="8" t="s">
         <v>11</v>
       </c>
       <c r="F6" s="8"/>
-      <c r="G6" s="6"/>
-      <c r="H6" s="11"/>
-      <c r="I6" s="18"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="12"/>
+      <c r="I6" s="19"/>
       <c r="J6" s="8"/>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="6"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="7"/>
+      <c r="B7" s="9"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="13"/>
       <c r="E7" s="8" t="s">
         <v>11</v>
       </c>
       <c r="F7" s="8"/>
-      <c r="G7" s="6"/>
-      <c r="H7" s="7"/>
-      <c r="I7" s="18"/>
+      <c r="G7" s="9"/>
+      <c r="H7" s="13"/>
+      <c r="I7" s="19"/>
       <c r="J7" s="8"/>
     </row>
     <row r="8" spans="1:10">
@@ -1312,14 +1336,14 @@
       </c>
       <c r="B8" s="8"/>
       <c r="C8" s="8"/>
-      <c r="D8" s="13"/>
+      <c r="D8" s="14"/>
       <c r="E8" s="8" t="s">
         <v>18</v>
       </c>
       <c r="F8" s="8"/>
       <c r="G8" s="8"/>
-      <c r="H8" s="13"/>
-      <c r="I8" s="18"/>
+      <c r="H8" s="14"/>
+      <c r="I8" s="19"/>
       <c r="J8" s="8"/>
     </row>
     <row r="9" spans="1:10">
@@ -1328,14 +1352,14 @@
       </c>
       <c r="B9" s="8"/>
       <c r="C9" s="8"/>
-      <c r="D9" s="13"/>
+      <c r="D9" s="14"/>
       <c r="E9" s="8" t="s">
         <v>18</v>
       </c>
       <c r="F9" s="8"/>
       <c r="G9" s="8"/>
-      <c r="H9" s="13"/>
-      <c r="I9" s="18"/>
+      <c r="H9" s="14"/>
+      <c r="I9" s="19"/>
       <c r="J9" s="8"/>
     </row>
     <row r="10" spans="1:10">
@@ -1344,14 +1368,14 @@
       </c>
       <c r="B10" s="8"/>
       <c r="C10" s="8"/>
-      <c r="D10" s="13"/>
+      <c r="D10" s="14"/>
       <c r="E10" s="8" t="s">
         <v>18</v>
       </c>
       <c r="F10" s="8"/>
       <c r="G10" s="8"/>
-      <c r="H10" s="13"/>
-      <c r="I10" s="18"/>
+      <c r="H10" s="14"/>
+      <c r="I10" s="19"/>
       <c r="J10" s="8"/>
     </row>
     <row r="11" spans="1:10">
@@ -1360,14 +1384,14 @@
       </c>
       <c r="B11" s="8"/>
       <c r="C11" s="8"/>
-      <c r="D11" s="13"/>
+      <c r="D11" s="14"/>
       <c r="E11" s="8" t="s">
         <v>11</v>
       </c>
       <c r="F11" s="8"/>
       <c r="G11" s="8"/>
-      <c r="H11" s="13"/>
-      <c r="I11" s="18"/>
+      <c r="H11" s="14"/>
+      <c r="I11" s="19"/>
       <c r="J11" s="8"/>
     </row>
     <row r="12" spans="1:10">
@@ -1376,14 +1400,14 @@
       </c>
       <c r="B12" s="8"/>
       <c r="C12" s="8"/>
-      <c r="D12" s="13"/>
+      <c r="D12" s="14"/>
       <c r="E12" s="8" t="s">
         <v>11</v>
       </c>
       <c r="F12" s="8"/>
       <c r="G12" s="8"/>
-      <c r="H12" s="13"/>
-      <c r="I12" s="18"/>
+      <c r="H12" s="14"/>
+      <c r="I12" s="19"/>
       <c r="J12" s="8"/>
     </row>
     <row r="13" spans="1:10">
@@ -1392,79 +1416,79 @@
       </c>
       <c r="B13" s="8"/>
       <c r="C13" s="8"/>
-      <c r="D13" s="13"/>
+      <c r="D13" s="14"/>
       <c r="E13" s="8" t="s">
         <v>18</v>
       </c>
       <c r="F13" s="8"/>
       <c r="G13" s="8"/>
-      <c r="H13" s="13"/>
-      <c r="I13" s="18"/>
+      <c r="H13" s="14"/>
+      <c r="I13" s="19"/>
       <c r="J13" s="8"/>
     </row>
     <row r="14" spans="1:10">
       <c r="A14" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B14" s="14"/>
-      <c r="C14" s="14"/>
-      <c r="D14" s="14"/>
+      <c r="B14" s="15"/>
+      <c r="C14" s="15"/>
+      <c r="D14" s="15"/>
       <c r="E14" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="F14" s="14"/>
-      <c r="G14" s="14"/>
-      <c r="H14" s="14"/>
-      <c r="I14" s="14"/>
-      <c r="J14" s="14"/>
+      <c r="F14" s="15"/>
+      <c r="G14" s="15"/>
+      <c r="H14" s="15"/>
+      <c r="I14" s="15"/>
+      <c r="J14" s="15"/>
     </row>
     <row r="15" spans="1:10">
       <c r="A15" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B15" s="14"/>
-      <c r="C15" s="14"/>
-      <c r="D15" s="14"/>
+      <c r="B15" s="15"/>
+      <c r="C15" s="15"/>
+      <c r="D15" s="15"/>
       <c r="E15" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="F15" s="14"/>
-      <c r="G15" s="14"/>
-      <c r="H15" s="14"/>
-      <c r="I15" s="14"/>
-      <c r="J15" s="14"/>
+      <c r="F15" s="15"/>
+      <c r="G15" s="15"/>
+      <c r="H15" s="15"/>
+      <c r="I15" s="15"/>
+      <c r="J15" s="15"/>
     </row>
     <row r="16" spans="1:10">
       <c r="A16" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B16" s="14"/>
-      <c r="C16" s="14"/>
-      <c r="D16" s="14"/>
+      <c r="B16" s="15"/>
+      <c r="C16" s="15"/>
+      <c r="D16" s="15"/>
       <c r="E16" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="F16" s="14"/>
-      <c r="G16" s="14"/>
-      <c r="H16" s="14"/>
-      <c r="I16" s="14"/>
-      <c r="J16" s="14"/>
+      <c r="F16" s="15"/>
+      <c r="G16" s="15"/>
+      <c r="H16" s="15"/>
+      <c r="I16" s="15"/>
+      <c r="J16" s="15"/>
     </row>
     <row r="17" spans="1:10">
       <c r="A17" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B17" s="15"/>
-      <c r="C17" s="15"/>
-      <c r="D17" s="15"/>
+      <c r="B17" s="16"/>
+      <c r="C17" s="16"/>
+      <c r="D17" s="16"/>
       <c r="E17" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="F17" s="15"/>
-      <c r="G17" s="15"/>
-      <c r="H17" s="15"/>
-      <c r="I17" s="15"/>
-      <c r="J17" s="15"/>
+      <c r="F17" s="16"/>
+      <c r="G17" s="16"/>
+      <c r="H17" s="16"/>
+      <c r="I17" s="16"/>
+      <c r="J17" s="16"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
Finished navbar, logo, banner, search modal without responsive
</commit_message>
<xml_diff>
--- a/Tasks.xlsx
+++ b/Tasks.xlsx
@@ -106,10 +106,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="25">
     <font>
@@ -159,8 +159,60 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -174,13 +226,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="18"/>
       <color theme="3"/>
@@ -189,85 +234,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -281,15 +250,46 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -328,19 +328,121 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -352,25 +454,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -382,85 +466,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -472,37 +502,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -540,7 +540,18 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -561,6 +572,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -576,28 +596,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -617,20 +620,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -639,15 +639,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -657,130 +657,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="20" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="22" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="14" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="14" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="25" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="28" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="28" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1167,7 +1167,7 @@
   <dimension ref="A1:M17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
@@ -1302,9 +1302,13 @@
       <c r="A6" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="6"/>
+      <c r="B6" s="6">
+        <v>45091</v>
+      </c>
       <c r="C6" s="6"/>
-      <c r="D6" s="12"/>
+      <c r="D6" s="12">
+        <v>0.6</v>
+      </c>
       <c r="E6" s="8" t="s">
         <v>11</v>
       </c>
@@ -1318,9 +1322,13 @@
       <c r="A7" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="9"/>
+      <c r="B7" s="6">
+        <v>45091</v>
+      </c>
       <c r="C7" s="9"/>
-      <c r="D7" s="13"/>
+      <c r="D7" s="12">
+        <v>0.6</v>
+      </c>
       <c r="E7" s="8" t="s">
         <v>11</v>
       </c>

</xml_diff>

<commit_message>
Style responsive for header and banner
</commit_message>
<xml_diff>
--- a/Tasks.xlsx
+++ b/Tasks.xlsx
@@ -106,9 +106,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="25">
@@ -159,6 +159,35 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
@@ -167,52 +196,41 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -226,17 +244,23 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -250,44 +274,20 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -328,25 +328,169 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -358,157 +502,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -537,11 +537,41 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -572,54 +602,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -634,12 +616,30 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -657,130 +657,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="20" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="23" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="15" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="25" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="28" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="28" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1167,7 +1167,7 @@
   <dimension ref="A1:M17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
@@ -1227,7 +1227,7 @@
       </c>
       <c r="C2" s="6"/>
       <c r="D2" s="7">
-        <v>0.6</v>
+        <v>0.9</v>
       </c>
       <c r="E2" s="8" t="s">
         <v>11</v>
@@ -1245,9 +1245,11 @@
       <c r="B3" s="6">
         <v>45090</v>
       </c>
-      <c r="C3" s="6"/>
+      <c r="C3" s="6">
+        <v>45092</v>
+      </c>
       <c r="D3" s="11">
-        <v>0.6</v>
+        <v>1</v>
       </c>
       <c r="E3" s="8" t="s">
         <v>11</v>
@@ -1266,8 +1268,8 @@
         <v>45090</v>
       </c>
       <c r="C4" s="6"/>
-      <c r="D4" s="12">
-        <v>0.6</v>
+      <c r="D4" s="7">
+        <v>0.9</v>
       </c>
       <c r="E4" s="8" t="s">
         <v>11</v>
@@ -1286,8 +1288,8 @@
         <v>45090</v>
       </c>
       <c r="C5" s="6"/>
-      <c r="D5" s="12">
-        <v>0.6</v>
+      <c r="D5" s="11">
+        <v>0.9</v>
       </c>
       <c r="E5" s="8" t="s">
         <v>11</v>
@@ -1305,9 +1307,11 @@
       <c r="B6" s="6">
         <v>45091</v>
       </c>
-      <c r="C6" s="6"/>
-      <c r="D6" s="12">
-        <v>0.6</v>
+      <c r="C6" s="6">
+        <v>45092</v>
+      </c>
+      <c r="D6" s="7">
+        <v>1</v>
       </c>
       <c r="E6" s="8" t="s">
         <v>11</v>
@@ -1325,9 +1329,11 @@
       <c r="B7" s="6">
         <v>45091</v>
       </c>
-      <c r="C7" s="9"/>
-      <c r="D7" s="12">
-        <v>0.6</v>
+      <c r="C7" s="6">
+        <v>45092</v>
+      </c>
+      <c r="D7" s="11">
+        <v>1</v>
       </c>
       <c r="E7" s="8" t="s">
         <v>11</v>

</xml_diff>

<commit_message>
Add new section (Blog, Q&A) + Update header
</commit_message>
<xml_diff>
--- a/Tasks.xlsx
+++ b/Tasks.xlsx
@@ -106,10 +106,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="25">
     <font>
@@ -141,12 +141,12 @@
     </font>
     <font>
       <sz val="10"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="134"/>
     </font>
     <font>
       <sz val="10"/>
-      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="134"/>
     </font>
@@ -159,6 +159,29 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
@@ -166,39 +189,31 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -212,55 +227,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -275,21 +244,52 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -328,13 +328,151 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -346,67 +484,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -418,97 +502,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -537,6 +537,30 @@
       <diagonal/>
     </border>
     <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -552,6 +576,24 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -563,41 +605,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -619,18 +626,11 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
+      <top style="thin">
         <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -639,15 +639,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -657,134 +657,134 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="15" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="28" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="28" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -806,28 +806,31 @@
     <xf numFmtId="16" fontId="3" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
+    <xf numFmtId="9" fontId="3" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="2" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="2" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="3" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
     <xf numFmtId="9" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1167,7 +1170,7 @@
   <dimension ref="A1:M17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
@@ -1208,13 +1211,13 @@
       <c r="H1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="17" t="s">
+      <c r="I1" s="18" t="s">
         <v>4</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="M1" s="18" t="s">
+      <c r="M1" s="19" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1225,9 +1228,11 @@
       <c r="B2" s="6">
         <v>45090</v>
       </c>
-      <c r="C2" s="6"/>
+      <c r="C2" s="6">
+        <v>45098</v>
+      </c>
       <c r="D2" s="7">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="E2" s="8" t="s">
         <v>11</v>
@@ -1235,7 +1240,7 @@
       <c r="F2" s="8"/>
       <c r="G2" s="9"/>
       <c r="H2" s="10"/>
-      <c r="I2" s="19"/>
+      <c r="I2" s="20"/>
       <c r="J2" s="8"/>
     </row>
     <row r="3" spans="1:10">
@@ -1248,7 +1253,7 @@
       <c r="C3" s="6">
         <v>45092</v>
       </c>
-      <c r="D3" s="11">
+      <c r="D3" s="7">
         <v>1</v>
       </c>
       <c r="E3" s="8" t="s">
@@ -1256,8 +1261,8 @@
       </c>
       <c r="F3" s="8"/>
       <c r="G3" s="9"/>
-      <c r="H3" s="11"/>
-      <c r="I3" s="19"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="20"/>
       <c r="J3" s="8"/>
     </row>
     <row r="4" spans="1:10">
@@ -1267,17 +1272,19 @@
       <c r="B4" s="6">
         <v>45090</v>
       </c>
-      <c r="C4" s="6"/>
+      <c r="C4" s="6">
+        <v>45098</v>
+      </c>
       <c r="D4" s="7">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="E4" s="8" t="s">
         <v>11</v>
       </c>
       <c r="F4" s="8"/>
       <c r="G4" s="9"/>
-      <c r="H4" s="12"/>
-      <c r="I4" s="19"/>
+      <c r="H4" s="11"/>
+      <c r="I4" s="20"/>
       <c r="J4" s="8"/>
     </row>
     <row r="5" spans="1:10">
@@ -1287,17 +1294,19 @@
       <c r="B5" s="6">
         <v>45090</v>
       </c>
-      <c r="C5" s="6"/>
-      <c r="D5" s="11">
-        <v>0.9</v>
+      <c r="C5" s="6">
+        <v>45098</v>
+      </c>
+      <c r="D5" s="7">
+        <v>1</v>
       </c>
       <c r="E5" s="8" t="s">
         <v>11</v>
       </c>
       <c r="F5" s="8"/>
       <c r="G5" s="9"/>
-      <c r="H5" s="13"/>
-      <c r="I5" s="19"/>
+      <c r="H5" s="12"/>
+      <c r="I5" s="20"/>
       <c r="J5" s="8"/>
     </row>
     <row r="6" spans="1:10">
@@ -1310,7 +1319,7 @@
       <c r="C6" s="6">
         <v>45092</v>
       </c>
-      <c r="D6" s="7">
+      <c r="D6" s="13">
         <v>1</v>
       </c>
       <c r="E6" s="8" t="s">
@@ -1318,8 +1327,8 @@
       </c>
       <c r="F6" s="8"/>
       <c r="G6" s="9"/>
-      <c r="H6" s="12"/>
-      <c r="I6" s="19"/>
+      <c r="H6" s="11"/>
+      <c r="I6" s="20"/>
       <c r="J6" s="8"/>
     </row>
     <row r="7" spans="1:10">
@@ -1332,7 +1341,7 @@
       <c r="C7" s="6">
         <v>45092</v>
       </c>
-      <c r="D7" s="11">
+      <c r="D7" s="7">
         <v>1</v>
       </c>
       <c r="E7" s="8" t="s">
@@ -1340,8 +1349,8 @@
       </c>
       <c r="F7" s="8"/>
       <c r="G7" s="9"/>
-      <c r="H7" s="13"/>
-      <c r="I7" s="19"/>
+      <c r="H7" s="12"/>
+      <c r="I7" s="20"/>
       <c r="J7" s="8"/>
     </row>
     <row r="8" spans="1:10">
@@ -1357,7 +1366,7 @@
       <c r="F8" s="8"/>
       <c r="G8" s="8"/>
       <c r="H8" s="14"/>
-      <c r="I8" s="19"/>
+      <c r="I8" s="20"/>
       <c r="J8" s="8"/>
     </row>
     <row r="9" spans="1:10">
@@ -1373,7 +1382,7 @@
       <c r="F9" s="8"/>
       <c r="G9" s="8"/>
       <c r="H9" s="14"/>
-      <c r="I9" s="19"/>
+      <c r="I9" s="20"/>
       <c r="J9" s="8"/>
     </row>
     <row r="10" spans="1:10">
@@ -1389,39 +1398,47 @@
       <c r="F10" s="8"/>
       <c r="G10" s="8"/>
       <c r="H10" s="14"/>
-      <c r="I10" s="19"/>
+      <c r="I10" s="20"/>
       <c r="J10" s="8"/>
     </row>
     <row r="11" spans="1:10">
       <c r="A11" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="8"/>
+      <c r="B11" s="6">
+        <v>45098</v>
+      </c>
       <c r="C11" s="8"/>
-      <c r="D11" s="14"/>
+      <c r="D11" s="15">
+        <v>0.9</v>
+      </c>
       <c r="E11" s="8" t="s">
         <v>11</v>
       </c>
       <c r="F11" s="8"/>
       <c r="G11" s="8"/>
       <c r="H11" s="14"/>
-      <c r="I11" s="19"/>
+      <c r="I11" s="20"/>
       <c r="J11" s="8"/>
     </row>
     <row r="12" spans="1:10">
       <c r="A12" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B12" s="8"/>
+      <c r="B12" s="6">
+        <v>45098</v>
+      </c>
       <c r="C12" s="8"/>
-      <c r="D12" s="14"/>
+      <c r="D12" s="15">
+        <v>0.8</v>
+      </c>
       <c r="E12" s="8" t="s">
         <v>11</v>
       </c>
       <c r="F12" s="8"/>
       <c r="G12" s="8"/>
       <c r="H12" s="14"/>
-      <c r="I12" s="19"/>
+      <c r="I12" s="20"/>
       <c r="J12" s="8"/>
     </row>
     <row r="13" spans="1:10">
@@ -1437,72 +1454,72 @@
       <c r="F13" s="8"/>
       <c r="G13" s="8"/>
       <c r="H13" s="14"/>
-      <c r="I13" s="19"/>
+      <c r="I13" s="20"/>
       <c r="J13" s="8"/>
     </row>
     <row r="14" spans="1:10">
       <c r="A14" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B14" s="15"/>
-      <c r="C14" s="15"/>
-      <c r="D14" s="15"/>
+      <c r="B14" s="6"/>
+      <c r="C14" s="16"/>
+      <c r="D14" s="16"/>
       <c r="E14" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="F14" s="15"/>
-      <c r="G14" s="15"/>
-      <c r="H14" s="15"/>
-      <c r="I14" s="15"/>
-      <c r="J14" s="15"/>
+      <c r="F14" s="16"/>
+      <c r="G14" s="16"/>
+      <c r="H14" s="16"/>
+      <c r="I14" s="16"/>
+      <c r="J14" s="16"/>
     </row>
     <row r="15" spans="1:10">
       <c r="A15" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B15" s="15"/>
-      <c r="C15" s="15"/>
-      <c r="D15" s="15"/>
+      <c r="B15" s="16"/>
+      <c r="C15" s="16"/>
+      <c r="D15" s="16"/>
       <c r="E15" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="F15" s="15"/>
-      <c r="G15" s="15"/>
-      <c r="H15" s="15"/>
-      <c r="I15" s="15"/>
-      <c r="J15" s="15"/>
+      <c r="F15" s="16"/>
+      <c r="G15" s="16"/>
+      <c r="H15" s="16"/>
+      <c r="I15" s="16"/>
+      <c r="J15" s="16"/>
     </row>
     <row r="16" spans="1:10">
       <c r="A16" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B16" s="15"/>
-      <c r="C16" s="15"/>
-      <c r="D16" s="15"/>
+      <c r="B16" s="16"/>
+      <c r="C16" s="16"/>
+      <c r="D16" s="16"/>
       <c r="E16" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="F16" s="15"/>
-      <c r="G16" s="15"/>
-      <c r="H16" s="15"/>
-      <c r="I16" s="15"/>
-      <c r="J16" s="15"/>
+      <c r="F16" s="16"/>
+      <c r="G16" s="16"/>
+      <c r="H16" s="16"/>
+      <c r="I16" s="16"/>
+      <c r="J16" s="16"/>
     </row>
     <row r="17" spans="1:10">
       <c r="A17" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B17" s="16"/>
-      <c r="C17" s="16"/>
-      <c r="D17" s="16"/>
+      <c r="B17" s="17"/>
+      <c r="C17" s="17"/>
+      <c r="D17" s="17"/>
       <c r="E17" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="F17" s="16"/>
-      <c r="G17" s="16"/>
-      <c r="H17" s="16"/>
-      <c r="I17" s="16"/>
-      <c r="J17" s="16"/>
+      <c r="F17" s="17"/>
+      <c r="G17" s="17"/>
+      <c r="H17" s="17"/>
+      <c r="I17" s="17"/>
+      <c r="J17" s="17"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
xong phan cua Hung
</commit_message>
<xml_diff>
--- a/Tasks.xlsx
+++ b/Tasks.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28125" windowHeight="12495"/>
+    <workbookView windowWidth="24225" windowHeight="12375"/>
   </bookViews>
   <sheets>
     <sheet name="Tasks" sheetId="1" r:id="rId1"/>
@@ -106,9 +106,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="25">
@@ -160,6 +160,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -167,30 +174,31 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -198,7 +206,22 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -212,84 +235,61 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -328,43 +328,157 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -376,97 +490,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -478,12 +502,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -491,24 +509,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -537,17 +537,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -567,6 +561,36 @@
       <diagonal/>
     </border>
     <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
@@ -578,26 +602,9 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
+      <top/>
       <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -619,18 +626,11 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
+      <top style="thin">
         <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -639,7 +639,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -660,131 +660,131 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="15" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="27" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="14" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -827,10 +827,22 @@
     <xf numFmtId="9" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
+    <xf numFmtId="16" fontId="3" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
@@ -1167,7 +1179,7 @@
   <dimension ref="A1:M17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
@@ -1208,13 +1220,13 @@
       <c r="H1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="17" t="s">
+      <c r="I1" s="21" t="s">
         <v>4</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="M1" s="18" t="s">
+      <c r="M1" s="22" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1235,7 +1247,7 @@
       <c r="F2" s="8"/>
       <c r="G2" s="9"/>
       <c r="H2" s="10"/>
-      <c r="I2" s="19"/>
+      <c r="I2" s="23"/>
       <c r="J2" s="8"/>
     </row>
     <row r="3" spans="1:10">
@@ -1257,7 +1269,7 @@
       <c r="F3" s="8"/>
       <c r="G3" s="9"/>
       <c r="H3" s="11"/>
-      <c r="I3" s="19"/>
+      <c r="I3" s="23"/>
       <c r="J3" s="8"/>
     </row>
     <row r="4" spans="1:10">
@@ -1277,7 +1289,7 @@
       <c r="F4" s="8"/>
       <c r="G4" s="9"/>
       <c r="H4" s="12"/>
-      <c r="I4" s="19"/>
+      <c r="I4" s="23"/>
       <c r="J4" s="8"/>
     </row>
     <row r="5" spans="1:10">
@@ -1297,7 +1309,7 @@
       <c r="F5" s="8"/>
       <c r="G5" s="9"/>
       <c r="H5" s="13"/>
-      <c r="I5" s="19"/>
+      <c r="I5" s="23"/>
       <c r="J5" s="8"/>
     </row>
     <row r="6" spans="1:10">
@@ -1319,7 +1331,7 @@
       <c r="F6" s="8"/>
       <c r="G6" s="9"/>
       <c r="H6" s="12"/>
-      <c r="I6" s="19"/>
+      <c r="I6" s="23"/>
       <c r="J6" s="8"/>
     </row>
     <row r="7" spans="1:10">
@@ -1341,55 +1353,73 @@
       <c r="F7" s="8"/>
       <c r="G7" s="9"/>
       <c r="H7" s="13"/>
-      <c r="I7" s="19"/>
+      <c r="I7" s="23"/>
       <c r="J7" s="8"/>
     </row>
     <row r="8" spans="1:10">
       <c r="A8" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="8"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="14"/>
+      <c r="B8" s="14">
+        <v>45098</v>
+      </c>
+      <c r="C8" s="14">
+        <v>45098</v>
+      </c>
+      <c r="D8" s="15">
+        <v>1</v>
+      </c>
       <c r="E8" s="8" t="s">
         <v>18</v>
       </c>
       <c r="F8" s="8"/>
       <c r="G8" s="8"/>
-      <c r="H8" s="14"/>
-      <c r="I8" s="19"/>
+      <c r="H8" s="16"/>
+      <c r="I8" s="23"/>
       <c r="J8" s="8"/>
     </row>
     <row r="9" spans="1:10">
       <c r="A9" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="8"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="14"/>
+      <c r="B9" s="14">
+        <v>45098</v>
+      </c>
+      <c r="C9" s="14">
+        <v>45098</v>
+      </c>
+      <c r="D9" s="15">
+        <v>1</v>
+      </c>
       <c r="E9" s="8" t="s">
         <v>18</v>
       </c>
       <c r="F9" s="8"/>
       <c r="G9" s="8"/>
-      <c r="H9" s="14"/>
-      <c r="I9" s="19"/>
+      <c r="H9" s="16"/>
+      <c r="I9" s="23"/>
       <c r="J9" s="8"/>
     </row>
     <row r="10" spans="1:10">
       <c r="A10" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="8"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="14"/>
+      <c r="B10" s="14">
+        <v>45098</v>
+      </c>
+      <c r="C10" s="14">
+        <v>45098</v>
+      </c>
+      <c r="D10" s="15">
+        <v>1</v>
+      </c>
       <c r="E10" s="8" t="s">
         <v>18</v>
       </c>
       <c r="F10" s="8"/>
       <c r="G10" s="8"/>
-      <c r="H10" s="14"/>
-      <c r="I10" s="19"/>
+      <c r="H10" s="16"/>
+      <c r="I10" s="23"/>
       <c r="J10" s="8"/>
     </row>
     <row r="11" spans="1:10">
@@ -1398,14 +1428,14 @@
       </c>
       <c r="B11" s="8"/>
       <c r="C11" s="8"/>
-      <c r="D11" s="14"/>
+      <c r="D11" s="16"/>
       <c r="E11" s="8" t="s">
         <v>11</v>
       </c>
       <c r="F11" s="8"/>
       <c r="G11" s="8"/>
-      <c r="H11" s="14"/>
-      <c r="I11" s="19"/>
+      <c r="H11" s="16"/>
+      <c r="I11" s="23"/>
       <c r="J11" s="8"/>
     </row>
     <row r="12" spans="1:10">
@@ -1414,95 +1444,111 @@
       </c>
       <c r="B12" s="8"/>
       <c r="C12" s="8"/>
-      <c r="D12" s="14"/>
+      <c r="D12" s="16"/>
       <c r="E12" s="8" t="s">
         <v>11</v>
       </c>
       <c r="F12" s="8"/>
       <c r="G12" s="8"/>
-      <c r="H12" s="14"/>
-      <c r="I12" s="19"/>
+      <c r="H12" s="16"/>
+      <c r="I12" s="23"/>
       <c r="J12" s="8"/>
     </row>
     <row r="13" spans="1:10">
       <c r="A13" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B13" s="8"/>
+      <c r="B13" s="14">
+        <v>45098</v>
+      </c>
       <c r="C13" s="8"/>
-      <c r="D13" s="14"/>
+      <c r="D13" s="15">
+        <v>0.9</v>
+      </c>
       <c r="E13" s="8" t="s">
         <v>18</v>
       </c>
       <c r="F13" s="8"/>
       <c r="G13" s="8"/>
-      <c r="H13" s="14"/>
-      <c r="I13" s="19"/>
+      <c r="H13" s="16"/>
+      <c r="I13" s="23"/>
       <c r="J13" s="8"/>
     </row>
     <row r="14" spans="1:10">
       <c r="A14" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B14" s="15"/>
-      <c r="C14" s="15"/>
-      <c r="D14" s="15"/>
+      <c r="B14" s="17"/>
+      <c r="C14" s="17"/>
+      <c r="D14" s="17"/>
       <c r="E14" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="F14" s="15"/>
-      <c r="G14" s="15"/>
-      <c r="H14" s="15"/>
-      <c r="I14" s="15"/>
-      <c r="J14" s="15"/>
+      <c r="F14" s="17"/>
+      <c r="G14" s="17"/>
+      <c r="H14" s="17"/>
+      <c r="I14" s="17"/>
+      <c r="J14" s="17"/>
     </row>
     <row r="15" spans="1:10">
       <c r="A15" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B15" s="15"/>
-      <c r="C15" s="15"/>
-      <c r="D15" s="15"/>
+      <c r="B15" s="18">
+        <v>45098</v>
+      </c>
+      <c r="C15" s="18">
+        <v>45101</v>
+      </c>
+      <c r="D15" s="19">
+        <v>1</v>
+      </c>
       <c r="E15" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="F15" s="15"/>
-      <c r="G15" s="15"/>
-      <c r="H15" s="15"/>
-      <c r="I15" s="15"/>
-      <c r="J15" s="15"/>
+      <c r="F15" s="17"/>
+      <c r="G15" s="17"/>
+      <c r="H15" s="17"/>
+      <c r="I15" s="17"/>
+      <c r="J15" s="17"/>
     </row>
     <row r="16" spans="1:10">
       <c r="A16" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B16" s="15"/>
-      <c r="C16" s="15"/>
-      <c r="D16" s="15"/>
+      <c r="B16" s="18">
+        <v>45098</v>
+      </c>
+      <c r="C16" s="18">
+        <v>45098</v>
+      </c>
+      <c r="D16" s="19">
+        <v>1</v>
+      </c>
       <c r="E16" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="F16" s="15"/>
-      <c r="G16" s="15"/>
-      <c r="H16" s="15"/>
-      <c r="I16" s="15"/>
-      <c r="J16" s="15"/>
+      <c r="F16" s="17"/>
+      <c r="G16" s="17"/>
+      <c r="H16" s="17"/>
+      <c r="I16" s="17"/>
+      <c r="J16" s="17"/>
     </row>
     <row r="17" spans="1:10">
       <c r="A17" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B17" s="16"/>
-      <c r="C17" s="16"/>
-      <c r="D17" s="16"/>
+      <c r="B17" s="20"/>
+      <c r="C17" s="20"/>
+      <c r="D17" s="20"/>
       <c r="E17" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="F17" s="16"/>
-      <c r="G17" s="16"/>
-      <c r="H17" s="16"/>
-      <c r="I17" s="16"/>
-      <c r="J17" s="16"/>
+      <c r="F17" s="20"/>
+      <c r="G17" s="20"/>
+      <c r="H17" s="20"/>
+      <c r="I17" s="20"/>
+      <c r="J17" s="20"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
My Anh commit Tasks.xlsx file
</commit_message>
<xml_diff>
--- a/Tasks.xlsx
+++ b/Tasks.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="24225" windowHeight="12375"/>
+    <workbookView windowWidth="28125" windowHeight="12495"/>
   </bookViews>
   <sheets>
     <sheet name="Tasks" sheetId="1" r:id="rId1"/>
@@ -141,40 +141,123 @@
     </font>
     <font>
       <sz val="10"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="134"/>
     </font>
     <font>
       <sz val="10"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF006100"/>
       <name val="Calibri"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -188,9 +271,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -198,98 +281,15 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -328,97 +328,175 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -430,85 +508,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -541,7 +541,22 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -561,17 +576,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -594,17 +603,19 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right/>
-      <top/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -623,23 +634,12 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -657,130 +657,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="17" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="19" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="31" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="31" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="27" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="14" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -806,24 +806,24 @@
     <xf numFmtId="16" fontId="3" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
+    <xf numFmtId="9" fontId="3" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="2" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="2" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="3" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
     <xf numFmtId="9" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
@@ -836,13 +836,13 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
@@ -1179,7 +1179,7 @@
   <dimension ref="A1:M17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
@@ -1237,9 +1237,11 @@
       <c r="B2" s="6">
         <v>45090</v>
       </c>
-      <c r="C2" s="6"/>
+      <c r="C2" s="6">
+        <v>45098</v>
+      </c>
       <c r="D2" s="7">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="E2" s="8" t="s">
         <v>11</v>
@@ -1260,7 +1262,7 @@
       <c r="C3" s="6">
         <v>45092</v>
       </c>
-      <c r="D3" s="11">
+      <c r="D3" s="7">
         <v>1</v>
       </c>
       <c r="E3" s="8" t="s">
@@ -1268,7 +1270,7 @@
       </c>
       <c r="F3" s="8"/>
       <c r="G3" s="9"/>
-      <c r="H3" s="11"/>
+      <c r="H3" s="7"/>
       <c r="I3" s="23"/>
       <c r="J3" s="8"/>
     </row>
@@ -1279,16 +1281,18 @@
       <c r="B4" s="6">
         <v>45090</v>
       </c>
-      <c r="C4" s="6"/>
+      <c r="C4" s="6">
+        <v>45098</v>
+      </c>
       <c r="D4" s="7">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="E4" s="8" t="s">
         <v>11</v>
       </c>
       <c r="F4" s="8"/>
       <c r="G4" s="9"/>
-      <c r="H4" s="12"/>
+      <c r="H4" s="11"/>
       <c r="I4" s="23"/>
       <c r="J4" s="8"/>
     </row>
@@ -1299,16 +1303,18 @@
       <c r="B5" s="6">
         <v>45090</v>
       </c>
-      <c r="C5" s="6"/>
-      <c r="D5" s="11">
-        <v>0.9</v>
+      <c r="C5" s="6">
+        <v>45098</v>
+      </c>
+      <c r="D5" s="7">
+        <v>1</v>
       </c>
       <c r="E5" s="8" t="s">
         <v>11</v>
       </c>
       <c r="F5" s="8"/>
       <c r="G5" s="9"/>
-      <c r="H5" s="13"/>
+      <c r="H5" s="12"/>
       <c r="I5" s="23"/>
       <c r="J5" s="8"/>
     </row>
@@ -1322,7 +1328,7 @@
       <c r="C6" s="6">
         <v>45092</v>
       </c>
-      <c r="D6" s="7">
+      <c r="D6" s="13">
         <v>1</v>
       </c>
       <c r="E6" s="8" t="s">
@@ -1330,7 +1336,7 @@
       </c>
       <c r="F6" s="8"/>
       <c r="G6" s="9"/>
-      <c r="H6" s="12"/>
+      <c r="H6" s="11"/>
       <c r="I6" s="23"/>
       <c r="J6" s="8"/>
     </row>
@@ -1344,7 +1350,7 @@
       <c r="C7" s="6">
         <v>45092</v>
       </c>
-      <c r="D7" s="11">
+      <c r="D7" s="7">
         <v>1</v>
       </c>
       <c r="E7" s="8" t="s">
@@ -1352,7 +1358,7 @@
       </c>
       <c r="F7" s="8"/>
       <c r="G7" s="9"/>
-      <c r="H7" s="13"/>
+      <c r="H7" s="12"/>
       <c r="I7" s="23"/>
       <c r="J7" s="8"/>
     </row>
@@ -1426,9 +1432,15 @@
       <c r="A11" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="8"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="16"/>
+      <c r="B11" s="6">
+        <v>45098</v>
+      </c>
+      <c r="C11" s="14">
+        <v>45106</v>
+      </c>
+      <c r="D11" s="15">
+        <v>1</v>
+      </c>
       <c r="E11" s="8" t="s">
         <v>11</v>
       </c>
@@ -1442,9 +1454,15 @@
       <c r="A12" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B12" s="8"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="16"/>
+      <c r="B12" s="6">
+        <v>45098</v>
+      </c>
+      <c r="C12" s="14">
+        <v>45106</v>
+      </c>
+      <c r="D12" s="15">
+        <v>1</v>
+      </c>
       <c r="E12" s="8" t="s">
         <v>11</v>
       </c>
@@ -1478,69 +1496,81 @@
       <c r="A14" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B14" s="17"/>
-      <c r="C14" s="17"/>
-      <c r="D14" s="17"/>
+      <c r="B14" s="6">
+        <v>45103</v>
+      </c>
+      <c r="C14" s="14">
+        <v>45106</v>
+      </c>
+      <c r="D14" s="17">
+        <v>1</v>
+      </c>
       <c r="E14" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="F14" s="17"/>
-      <c r="G14" s="17"/>
-      <c r="H14" s="17"/>
-      <c r="I14" s="17"/>
-      <c r="J14" s="17"/>
+      <c r="F14" s="18"/>
+      <c r="G14" s="18"/>
+      <c r="H14" s="18"/>
+      <c r="I14" s="18"/>
+      <c r="J14" s="18"/>
     </row>
     <row r="15" spans="1:10">
       <c r="A15" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B15" s="18">
+      <c r="B15" s="19">
         <v>45098</v>
       </c>
-      <c r="C15" s="18">
+      <c r="C15" s="19">
         <v>45101</v>
       </c>
-      <c r="D15" s="19">
+      <c r="D15" s="17">
         <v>1</v>
       </c>
       <c r="E15" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="F15" s="17"/>
-      <c r="G15" s="17"/>
-      <c r="H15" s="17"/>
-      <c r="I15" s="17"/>
-      <c r="J15" s="17"/>
+      <c r="F15" s="18"/>
+      <c r="G15" s="18"/>
+      <c r="H15" s="18"/>
+      <c r="I15" s="18"/>
+      <c r="J15" s="18"/>
     </row>
     <row r="16" spans="1:10">
       <c r="A16" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B16" s="18">
+      <c r="B16" s="19">
         <v>45098</v>
       </c>
-      <c r="C16" s="18">
+      <c r="C16" s="19">
         <v>45098</v>
       </c>
-      <c r="D16" s="19">
+      <c r="D16" s="17">
         <v>1</v>
       </c>
       <c r="E16" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="F16" s="17"/>
-      <c r="G16" s="17"/>
-      <c r="H16" s="17"/>
-      <c r="I16" s="17"/>
-      <c r="J16" s="17"/>
+      <c r="F16" s="18"/>
+      <c r="G16" s="18"/>
+      <c r="H16" s="18"/>
+      <c r="I16" s="18"/>
+      <c r="J16" s="18"/>
     </row>
     <row r="17" spans="1:10">
       <c r="A17" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B17" s="20"/>
-      <c r="C17" s="20"/>
-      <c r="D17" s="20"/>
+      <c r="B17" s="6">
+        <v>45103</v>
+      </c>
+      <c r="C17" s="14">
+        <v>45106</v>
+      </c>
+      <c r="D17" s="17">
+        <v>1</v>
+      </c>
       <c r="E17" s="8" t="s">
         <v>11</v>
       </c>

</xml_diff>